<commit_message>
Klassen umbenannt, PreparedStatement eingefügt
</commit_message>
<xml_diff>
--- a/bin/input_output_Excel/OUTPUT_Mappe_Personen.xlsx
+++ b/bin/input_output_Excel/OUTPUT_Mappe_Personen.xlsx
@@ -1299,7 +1299,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="n">
-        <v>21.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="3">
@@ -1313,7 +1313,7 @@
         <v>7</v>
       </c>
       <c r="D3" t="n">
-        <v>25.0</v>
+        <v>48.0</v>
       </c>
     </row>
     <row r="4">
@@ -1327,7 +1327,7 @@
         <v>9</v>
       </c>
       <c r="D4" t="n">
-        <v>33.0</v>
+        <v>31.0</v>
       </c>
     </row>
     <row r="5">
@@ -1341,7 +1341,7 @@
         <v>11</v>
       </c>
       <c r="D5" t="n">
-        <v>35.0</v>
+        <v>59.0</v>
       </c>
     </row>
     <row r="6">
@@ -1355,7 +1355,7 @@
         <v>13</v>
       </c>
       <c r="D6" t="n">
-        <v>67.0</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="7">
@@ -1369,7 +1369,7 @@
         <v>15</v>
       </c>
       <c r="D7" t="n">
-        <v>58.0</v>
+        <v>55.0</v>
       </c>
     </row>
     <row r="8">
@@ -1383,7 +1383,7 @@
         <v>17</v>
       </c>
       <c r="D8" t="n">
-        <v>35.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="9">
@@ -1397,7 +1397,7 @@
         <v>19</v>
       </c>
       <c r="D9" t="n">
-        <v>29.0</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="10">
@@ -1411,7 +1411,7 @@
         <v>21</v>
       </c>
       <c r="D10" t="n">
-        <v>39.0</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="11">
@@ -1425,7 +1425,7 @@
         <v>23</v>
       </c>
       <c r="D11" t="n">
-        <v>50.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="12">
@@ -1439,7 +1439,7 @@
         <v>25</v>
       </c>
       <c r="D12" t="n">
-        <v>52.0</v>
+        <v>29.0</v>
       </c>
     </row>
     <row r="13">
@@ -1453,7 +1453,7 @@
         <v>27</v>
       </c>
       <c r="D13" t="n">
-        <v>40.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="14">
@@ -1467,7 +1467,7 @@
         <v>29</v>
       </c>
       <c r="D14" t="n">
-        <v>47.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="15">
@@ -1481,7 +1481,7 @@
         <v>31</v>
       </c>
       <c r="D15" t="n">
-        <v>43.0</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="16">
@@ -1495,7 +1495,7 @@
         <v>33</v>
       </c>
       <c r="D16" t="n">
-        <v>47.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="17">
@@ -1509,7 +1509,7 @@
         <v>35</v>
       </c>
       <c r="D17" t="n">
-        <v>33.0</v>
+        <v>29.0</v>
       </c>
     </row>
     <row r="18">
@@ -1523,7 +1523,7 @@
         <v>37</v>
       </c>
       <c r="D18" t="n">
-        <v>62.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="19">
@@ -1537,7 +1537,7 @@
         <v>39</v>
       </c>
       <c r="D19" t="n">
-        <v>60.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="20">
@@ -1551,7 +1551,7 @@
         <v>41</v>
       </c>
       <c r="D20" t="n">
-        <v>55.0</v>
+        <v>44.0</v>
       </c>
     </row>
     <row r="21">
@@ -1565,7 +1565,7 @@
         <v>43</v>
       </c>
       <c r="D21" t="n">
-        <v>48.0</v>
+        <v>66.0</v>
       </c>
     </row>
     <row r="22">
@@ -1579,7 +1579,7 @@
         <v>45</v>
       </c>
       <c r="D22" t="n">
-        <v>27.0</v>
+        <v>65.0</v>
       </c>
     </row>
     <row r="23">
@@ -1593,7 +1593,7 @@
         <v>47</v>
       </c>
       <c r="D23" t="n">
-        <v>59.0</v>
+        <v>38.0</v>
       </c>
     </row>
     <row r="24">
@@ -1607,7 +1607,7 @@
         <v>49</v>
       </c>
       <c r="D24" t="n">
-        <v>24.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="25">
@@ -1621,7 +1621,7 @@
         <v>51</v>
       </c>
       <c r="D25" t="n">
-        <v>62.0</v>
+        <v>53.0</v>
       </c>
     </row>
     <row r="26">
@@ -1635,7 +1635,7 @@
         <v>53</v>
       </c>
       <c r="D26" t="n">
-        <v>27.0</v>
+        <v>31.0</v>
       </c>
     </row>
     <row r="27">
@@ -1649,7 +1649,7 @@
         <v>55</v>
       </c>
       <c r="D27" t="n">
-        <v>27.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="28">
@@ -1663,7 +1663,7 @@
         <v>57</v>
       </c>
       <c r="D28" t="n">
-        <v>53.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="29">
@@ -1677,7 +1677,7 @@
         <v>59</v>
       </c>
       <c r="D29" t="n">
-        <v>65.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="30">
@@ -1691,7 +1691,7 @@
         <v>61</v>
       </c>
       <c r="D30" t="n">
-        <v>51.0</v>
+        <v>29.0</v>
       </c>
     </row>
     <row r="31">
@@ -1705,7 +1705,7 @@
         <v>63</v>
       </c>
       <c r="D31" t="n">
-        <v>44.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="32">
@@ -1719,7 +1719,7 @@
         <v>65</v>
       </c>
       <c r="D32" t="n">
-        <v>40.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="33">
@@ -1733,7 +1733,7 @@
         <v>67</v>
       </c>
       <c r="D33" t="n">
-        <v>33.0</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="34">
@@ -1747,7 +1747,7 @@
         <v>69</v>
       </c>
       <c r="D34" t="n">
-        <v>61.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="35">
@@ -1761,7 +1761,7 @@
         <v>71</v>
       </c>
       <c r="D35" t="n">
-        <v>62.0</v>
+        <v>42.0</v>
       </c>
     </row>
     <row r="36">
@@ -1775,7 +1775,7 @@
         <v>73</v>
       </c>
       <c r="D36" t="n">
-        <v>41.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="37">
@@ -1789,7 +1789,7 @@
         <v>75</v>
       </c>
       <c r="D37" t="n">
-        <v>30.0</v>
+        <v>29.0</v>
       </c>
     </row>
     <row r="38">
@@ -1803,7 +1803,7 @@
         <v>77</v>
       </c>
       <c r="D38" t="n">
-        <v>31.0</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="39">
@@ -1817,7 +1817,7 @@
         <v>79</v>
       </c>
       <c r="D39" t="n">
-        <v>37.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="40">
@@ -1831,7 +1831,7 @@
         <v>81</v>
       </c>
       <c r="D40" t="n">
-        <v>26.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="41">
@@ -1845,7 +1845,7 @@
         <v>83</v>
       </c>
       <c r="D41" t="n">
-        <v>48.0</v>
+        <v>65.0</v>
       </c>
     </row>
     <row r="42">
@@ -1859,7 +1859,7 @@
         <v>85</v>
       </c>
       <c r="D42" t="n">
-        <v>19.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="43">
@@ -1873,7 +1873,7 @@
         <v>87</v>
       </c>
       <c r="D43" t="n">
-        <v>30.0</v>
+        <v>43.0</v>
       </c>
     </row>
     <row r="44">
@@ -1887,7 +1887,7 @@
         <v>89</v>
       </c>
       <c r="D44" t="n">
-        <v>39.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="45">
@@ -1901,7 +1901,7 @@
         <v>91</v>
       </c>
       <c r="D45" t="n">
-        <v>26.0</v>
+        <v>49.0</v>
       </c>
     </row>
     <row r="46">
@@ -1915,7 +1915,7 @@
         <v>93</v>
       </c>
       <c r="D46" t="n">
-        <v>50.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="47">
@@ -1929,7 +1929,7 @@
         <v>95</v>
       </c>
       <c r="D47" t="n">
-        <v>44.0</v>
+        <v>43.0</v>
       </c>
     </row>
     <row r="48">
@@ -1943,7 +1943,7 @@
         <v>97</v>
       </c>
       <c r="D48" t="n">
-        <v>60.0</v>
+        <v>18.0</v>
       </c>
     </row>
     <row r="49">
@@ -1957,7 +1957,7 @@
         <v>99</v>
       </c>
       <c r="D49" t="n">
-        <v>63.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="50">
@@ -1971,7 +1971,7 @@
         <v>101</v>
       </c>
       <c r="D50" t="n">
-        <v>20.0</v>
+        <v>53.0</v>
       </c>
     </row>
     <row r="51">
@@ -1985,7 +1985,7 @@
         <v>103</v>
       </c>
       <c r="D51" t="n">
-        <v>39.0</v>
+        <v>41.0</v>
       </c>
     </row>
     <row r="52">
@@ -1999,7 +1999,7 @@
         <v>105</v>
       </c>
       <c r="D52" t="n">
-        <v>46.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="53">
@@ -2013,7 +2013,7 @@
         <v>107</v>
       </c>
       <c r="D53" t="n">
-        <v>44.0</v>
+        <v>37.0</v>
       </c>
     </row>
     <row r="54">
@@ -2027,7 +2027,7 @@
         <v>109</v>
       </c>
       <c r="D54" t="n">
-        <v>60.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="55">
@@ -2041,7 +2041,7 @@
         <v>111</v>
       </c>
       <c r="D55" t="n">
-        <v>21.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="56">
@@ -2055,7 +2055,7 @@
         <v>113</v>
       </c>
       <c r="D56" t="n">
-        <v>44.0</v>
+        <v>54.0</v>
       </c>
     </row>
     <row r="57">
@@ -2069,7 +2069,7 @@
         <v>115</v>
       </c>
       <c r="D57" t="n">
-        <v>59.0</v>
+        <v>53.0</v>
       </c>
     </row>
     <row r="58">
@@ -2083,7 +2083,7 @@
         <v>117</v>
       </c>
       <c r="D58" t="n">
-        <v>25.0</v>
+        <v>67.0</v>
       </c>
     </row>
     <row r="59">
@@ -2097,7 +2097,7 @@
         <v>119</v>
       </c>
       <c r="D59" t="n">
-        <v>57.0</v>
+        <v>47.0</v>
       </c>
     </row>
     <row r="60">
@@ -2111,7 +2111,7 @@
         <v>121</v>
       </c>
       <c r="D60" t="n">
-        <v>24.0</v>
+        <v>47.0</v>
       </c>
     </row>
     <row r="61">
@@ -2125,7 +2125,7 @@
         <v>123</v>
       </c>
       <c r="D61" t="n">
-        <v>67.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="62">
@@ -2139,7 +2139,7 @@
         <v>125</v>
       </c>
       <c r="D62" t="n">
-        <v>22.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="63">
@@ -2153,7 +2153,7 @@
         <v>127</v>
       </c>
       <c r="D63" t="n">
-        <v>60.0</v>
+        <v>57.0</v>
       </c>
     </row>
     <row r="64">
@@ -2167,7 +2167,7 @@
         <v>129</v>
       </c>
       <c r="D64" t="n">
-        <v>43.0</v>
+        <v>57.0</v>
       </c>
     </row>
     <row r="65">
@@ -2181,7 +2181,7 @@
         <v>131</v>
       </c>
       <c r="D65" t="n">
-        <v>28.0</v>
+        <v>59.0</v>
       </c>
     </row>
     <row r="66">
@@ -2195,7 +2195,7 @@
         <v>133</v>
       </c>
       <c r="D66" t="n">
-        <v>31.0</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="67">
@@ -2209,7 +2209,7 @@
         <v>135</v>
       </c>
       <c r="D67" t="n">
-        <v>58.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="68">
@@ -2223,7 +2223,7 @@
         <v>137</v>
       </c>
       <c r="D68" t="n">
-        <v>24.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="69">
@@ -2237,7 +2237,7 @@
         <v>139</v>
       </c>
       <c r="D69" t="n">
-        <v>27.0</v>
+        <v>65.0</v>
       </c>
     </row>
     <row r="70">
@@ -2251,7 +2251,7 @@
         <v>141</v>
       </c>
       <c r="D70" t="n">
-        <v>29.0</v>
+        <v>51.0</v>
       </c>
     </row>
     <row r="71">
@@ -2265,7 +2265,7 @@
         <v>143</v>
       </c>
       <c r="D71" t="n">
-        <v>50.0</v>
+        <v>66.0</v>
       </c>
     </row>
     <row r="72">
@@ -2279,7 +2279,7 @@
         <v>145</v>
       </c>
       <c r="D72" t="n">
-        <v>44.0</v>
+        <v>48.0</v>
       </c>
     </row>
     <row r="73">
@@ -2293,7 +2293,7 @@
         <v>147</v>
       </c>
       <c r="D73" t="n">
-        <v>27.0</v>
+        <v>52.0</v>
       </c>
     </row>
     <row r="74">
@@ -2307,7 +2307,7 @@
         <v>149</v>
       </c>
       <c r="D74" t="n">
-        <v>30.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="75">
@@ -2321,7 +2321,7 @@
         <v>151</v>
       </c>
       <c r="D75" t="n">
-        <v>31.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="76">
@@ -2335,7 +2335,7 @@
         <v>153</v>
       </c>
       <c r="D76" t="n">
-        <v>41.0</v>
+        <v>64.0</v>
       </c>
     </row>
     <row r="77">
@@ -2349,7 +2349,7 @@
         <v>155</v>
       </c>
       <c r="D77" t="n">
-        <v>63.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="78">
@@ -2363,7 +2363,7 @@
         <v>157</v>
       </c>
       <c r="D78" t="n">
-        <v>33.0</v>
+        <v>27.0</v>
       </c>
     </row>
     <row r="79">
@@ -2377,7 +2377,7 @@
         <v>159</v>
       </c>
       <c r="D79" t="n">
-        <v>56.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="80">
@@ -2391,7 +2391,7 @@
         <v>161</v>
       </c>
       <c r="D80" t="n">
-        <v>51.0</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="81">
@@ -2405,7 +2405,7 @@
         <v>163</v>
       </c>
       <c r="D81" t="n">
-        <v>25.0</v>
+        <v>48.0</v>
       </c>
     </row>
     <row r="82">
@@ -2419,7 +2419,7 @@
         <v>165</v>
       </c>
       <c r="D82" t="n">
-        <v>21.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="83">
@@ -2433,7 +2433,7 @@
         <v>167</v>
       </c>
       <c r="D83" t="n">
-        <v>30.0</v>
+        <v>65.0</v>
       </c>
     </row>
     <row r="84">
@@ -2447,7 +2447,7 @@
         <v>169</v>
       </c>
       <c r="D84" t="n">
-        <v>55.0</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="85">
@@ -2461,7 +2461,7 @@
         <v>171</v>
       </c>
       <c r="D85" t="n">
-        <v>31.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="86">
@@ -2475,7 +2475,7 @@
         <v>173</v>
       </c>
       <c r="D86" t="n">
-        <v>59.0</v>
+        <v>63.0</v>
       </c>
     </row>
     <row r="87">
@@ -2489,7 +2489,7 @@
         <v>175</v>
       </c>
       <c r="D87" t="n">
-        <v>32.0</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="88">
@@ -2503,7 +2503,7 @@
         <v>177</v>
       </c>
       <c r="D88" t="n">
-        <v>34.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="89">
@@ -2517,7 +2517,7 @@
         <v>179</v>
       </c>
       <c r="D89" t="n">
-        <v>37.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="90">
@@ -2531,7 +2531,7 @@
         <v>181</v>
       </c>
       <c r="D90" t="n">
-        <v>32.0</v>
+        <v>20.0</v>
       </c>
     </row>
     <row r="91">
@@ -2545,7 +2545,7 @@
         <v>183</v>
       </c>
       <c r="D91" t="n">
-        <v>60.0</v>
+        <v>44.0</v>
       </c>
     </row>
     <row r="92">
@@ -2559,7 +2559,7 @@
         <v>185</v>
       </c>
       <c r="D92" t="n">
-        <v>52.0</v>
+        <v>49.0</v>
       </c>
     </row>
     <row r="93">
@@ -2573,7 +2573,7 @@
         <v>187</v>
       </c>
       <c r="D93" t="n">
-        <v>30.0</v>
+        <v>53.0</v>
       </c>
     </row>
     <row r="94">
@@ -2587,7 +2587,7 @@
         <v>189</v>
       </c>
       <c r="D94" t="n">
-        <v>53.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="95">
@@ -2601,7 +2601,7 @@
         <v>191</v>
       </c>
       <c r="D95" t="n">
-        <v>67.0</v>
+        <v>34.0</v>
       </c>
     </row>
     <row r="96">
@@ -2615,7 +2615,7 @@
         <v>193</v>
       </c>
       <c r="D96" t="n">
-        <v>63.0</v>
+        <v>43.0</v>
       </c>
     </row>
     <row r="97">
@@ -2629,7 +2629,7 @@
         <v>195</v>
       </c>
       <c r="D97" t="n">
-        <v>58.0</v>
+        <v>65.0</v>
       </c>
     </row>
     <row r="98">
@@ -2643,7 +2643,7 @@
         <v>197</v>
       </c>
       <c r="D98" t="n">
-        <v>27.0</v>
+        <v>54.0</v>
       </c>
     </row>
     <row r="99">
@@ -2657,7 +2657,7 @@
         <v>199</v>
       </c>
       <c r="D99" t="n">
-        <v>34.0</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="100">
@@ -2671,7 +2671,7 @@
         <v>201</v>
       </c>
       <c r="D100" t="n">
-        <v>41.0</v>
+        <v>33.0</v>
       </c>
     </row>
     <row r="101">
@@ -2685,7 +2685,7 @@
         <v>203</v>
       </c>
       <c r="D101" t="n">
-        <v>34.0</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="102">
@@ -2699,7 +2699,7 @@
         <v>205</v>
       </c>
       <c r="D102" t="n">
-        <v>42.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="103">
@@ -2713,7 +2713,7 @@
         <v>207</v>
       </c>
       <c r="D103" t="n">
-        <v>46.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="104">
@@ -2727,7 +2727,7 @@
         <v>209</v>
       </c>
       <c r="D104" t="n">
-        <v>39.0</v>
+        <v>49.0</v>
       </c>
     </row>
     <row r="105">
@@ -2741,7 +2741,7 @@
         <v>211</v>
       </c>
       <c r="D105" t="n">
-        <v>54.0</v>
+        <v>63.0</v>
       </c>
     </row>
     <row r="106">
@@ -2755,7 +2755,7 @@
         <v>213</v>
       </c>
       <c r="D106" t="n">
-        <v>57.0</v>
+        <v>60.0</v>
       </c>
     </row>
     <row r="107">
@@ -2769,7 +2769,7 @@
         <v>215</v>
       </c>
       <c r="D107" t="n">
-        <v>33.0</v>
+        <v>59.0</v>
       </c>
     </row>
     <row r="108">
@@ -2783,7 +2783,7 @@
         <v>217</v>
       </c>
       <c r="D108" t="n">
-        <v>52.0</v>
+        <v>41.0</v>
       </c>
     </row>
     <row r="109">
@@ -2797,7 +2797,7 @@
         <v>219</v>
       </c>
       <c r="D109" t="n">
-        <v>27.0</v>
+        <v>62.0</v>
       </c>
     </row>
     <row r="110">
@@ -2811,7 +2811,7 @@
         <v>221</v>
       </c>
       <c r="D110" t="n">
-        <v>43.0</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="111">
@@ -2825,7 +2825,7 @@
         <v>223</v>
       </c>
       <c r="D111" t="n">
-        <v>27.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="112">
@@ -2839,7 +2839,7 @@
         <v>225</v>
       </c>
       <c r="D112" t="n">
-        <v>44.0</v>
+        <v>46.0</v>
       </c>
     </row>
     <row r="113">
@@ -2853,7 +2853,7 @@
         <v>227</v>
       </c>
       <c r="D113" t="n">
-        <v>40.0</v>
+        <v>38.0</v>
       </c>
     </row>
     <row r="114">
@@ -2867,7 +2867,7 @@
         <v>229</v>
       </c>
       <c r="D114" t="n">
-        <v>41.0</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="115">
@@ -2881,7 +2881,7 @@
         <v>231</v>
       </c>
       <c r="D115" t="n">
-        <v>44.0</v>
+        <v>41.0</v>
       </c>
     </row>
     <row r="116">
@@ -2895,7 +2895,7 @@
         <v>233</v>
       </c>
       <c r="D116" t="n">
-        <v>46.0</v>
+        <v>65.0</v>
       </c>
     </row>
     <row r="117">
@@ -2909,7 +2909,7 @@
         <v>235</v>
       </c>
       <c r="D117" t="n">
-        <v>50.0</v>
+        <v>62.0</v>
       </c>
     </row>
     <row r="118">
@@ -2923,7 +2923,7 @@
         <v>237</v>
       </c>
       <c r="D118" t="n">
-        <v>43.0</v>
+        <v>52.0</v>
       </c>
     </row>
     <row r="119">
@@ -2937,7 +2937,7 @@
         <v>239</v>
       </c>
       <c r="D119" t="n">
-        <v>39.0</v>
+        <v>51.0</v>
       </c>
     </row>
     <row r="120">
@@ -2951,7 +2951,7 @@
         <v>241</v>
       </c>
       <c r="D120" t="n">
-        <v>55.0</v>
+        <v>57.0</v>
       </c>
     </row>
     <row r="121">
@@ -2965,7 +2965,7 @@
         <v>243</v>
       </c>
       <c r="D121" t="n">
-        <v>53.0</v>
+        <v>51.0</v>
       </c>
     </row>
     <row r="122">
@@ -2979,7 +2979,7 @@
         <v>245</v>
       </c>
       <c r="D122" t="n">
-        <v>28.0</v>
+        <v>62.0</v>
       </c>
     </row>
     <row r="123">
@@ -2993,7 +2993,7 @@
         <v>247</v>
       </c>
       <c r="D123" t="n">
-        <v>30.0</v>
+        <v>67.0</v>
       </c>
     </row>
     <row r="124">
@@ -3007,7 +3007,7 @@
         <v>249</v>
       </c>
       <c r="D124" t="n">
-        <v>51.0</v>
+        <v>42.0</v>
       </c>
     </row>
     <row r="125">
@@ -3035,7 +3035,7 @@
         <v>253</v>
       </c>
       <c r="D126" t="n">
-        <v>67.0</v>
+        <v>58.0</v>
       </c>
     </row>
     <row r="127">
@@ -3049,7 +3049,7 @@
         <v>255</v>
       </c>
       <c r="D127" t="n">
-        <v>56.0</v>
+        <v>44.0</v>
       </c>
     </row>
     <row r="128">
@@ -3063,7 +3063,7 @@
         <v>257</v>
       </c>
       <c r="D128" t="n">
-        <v>22.0</v>
+        <v>29.0</v>
       </c>
     </row>
     <row r="129">
@@ -3077,7 +3077,7 @@
         <v>259</v>
       </c>
       <c r="D129" t="n">
-        <v>21.0</v>
+        <v>63.0</v>
       </c>
     </row>
     <row r="130">
@@ -3091,7 +3091,7 @@
         <v>261</v>
       </c>
       <c r="D130" t="n">
-        <v>60.0</v>
+        <v>37.0</v>
       </c>
     </row>
     <row r="131">
@@ -3105,7 +3105,7 @@
         <v>263</v>
       </c>
       <c r="D131" t="n">
-        <v>22.0</v>
+        <v>38.0</v>
       </c>
     </row>
     <row r="132">
@@ -3119,7 +3119,7 @@
         <v>265</v>
       </c>
       <c r="D132" t="n">
-        <v>56.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="133">
@@ -3133,7 +3133,7 @@
         <v>267</v>
       </c>
       <c r="D133" t="n">
-        <v>33.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="134">
@@ -3147,7 +3147,7 @@
         <v>269</v>
       </c>
       <c r="D134" t="n">
-        <v>54.0</v>
+        <v>33.0</v>
       </c>
     </row>
     <row r="135">
@@ -3161,7 +3161,7 @@
         <v>271</v>
       </c>
       <c r="D135" t="n">
-        <v>26.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="136">
@@ -3175,7 +3175,7 @@
         <v>273</v>
       </c>
       <c r="D136" t="n">
-        <v>52.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="137">
@@ -3189,7 +3189,7 @@
         <v>275</v>
       </c>
       <c r="D137" t="n">
-        <v>27.0</v>
+        <v>59.0</v>
       </c>
     </row>
     <row r="138">
@@ -3203,7 +3203,7 @@
         <v>277</v>
       </c>
       <c r="D138" t="n">
-        <v>19.0</v>
+        <v>67.0</v>
       </c>
     </row>
     <row r="139">
@@ -3231,7 +3231,7 @@
         <v>281</v>
       </c>
       <c r="D140" t="n">
-        <v>66.0</v>
+        <v>59.0</v>
       </c>
     </row>
     <row r="141">
@@ -3245,7 +3245,7 @@
         <v>283</v>
       </c>
       <c r="D141" t="n">
-        <v>29.0</v>
+        <v>52.0</v>
       </c>
     </row>
     <row r="142">
@@ -3259,7 +3259,7 @@
         <v>285</v>
       </c>
       <c r="D142" t="n">
-        <v>52.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="143">
@@ -3273,7 +3273,7 @@
         <v>287</v>
       </c>
       <c r="D143" t="n">
-        <v>51.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="144">
@@ -3287,7 +3287,7 @@
         <v>289</v>
       </c>
       <c r="D144" t="n">
-        <v>44.0</v>
+        <v>34.0</v>
       </c>
     </row>
     <row r="145">
@@ -3301,7 +3301,7 @@
         <v>291</v>
       </c>
       <c r="D145" t="n">
-        <v>30.0</v>
+        <v>58.0</v>
       </c>
     </row>
     <row r="146">
@@ -3315,7 +3315,7 @@
         <v>293</v>
       </c>
       <c r="D146" t="n">
-        <v>27.0</v>
+        <v>37.0</v>
       </c>
     </row>
     <row r="147">
@@ -3329,7 +3329,7 @@
         <v>295</v>
       </c>
       <c r="D147" t="n">
-        <v>31.0</v>
+        <v>24.0</v>
       </c>
     </row>
     <row r="148">
@@ -3343,7 +3343,7 @@
         <v>297</v>
       </c>
       <c r="D148" t="n">
-        <v>48.0</v>
+        <v>53.0</v>
       </c>
     </row>
     <row r="149">
@@ -3357,7 +3357,7 @@
         <v>299</v>
       </c>
       <c r="D149" t="n">
-        <v>45.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="150">
@@ -3371,7 +3371,7 @@
         <v>301</v>
       </c>
       <c r="D150" t="n">
-        <v>22.0</v>
+        <v>42.0</v>
       </c>
     </row>
     <row r="151">
@@ -3385,7 +3385,7 @@
         <v>303</v>
       </c>
       <c r="D151" t="n">
-        <v>25.0</v>
+        <v>44.0</v>
       </c>
     </row>
     <row r="152">
@@ -3399,7 +3399,7 @@
         <v>305</v>
       </c>
       <c r="D152" t="n">
-        <v>48.0</v>
+        <v>32.0</v>
       </c>
     </row>
     <row r="153">
@@ -3413,7 +3413,7 @@
         <v>307</v>
       </c>
       <c r="D153" t="n">
-        <v>31.0</v>
+        <v>66.0</v>
       </c>
     </row>
     <row r="154">
@@ -3427,7 +3427,7 @@
         <v>309</v>
       </c>
       <c r="D154" t="n">
-        <v>38.0</v>
+        <v>62.0</v>
       </c>
     </row>
     <row r="155">
@@ -3441,7 +3441,7 @@
         <v>311</v>
       </c>
       <c r="D155" t="n">
-        <v>26.0</v>
+        <v>67.0</v>
       </c>
     </row>
     <row r="156">
@@ -3469,7 +3469,7 @@
         <v>315</v>
       </c>
       <c r="D157" t="n">
-        <v>61.0</v>
+        <v>31.0</v>
       </c>
     </row>
     <row r="158">
@@ -3483,7 +3483,7 @@
         <v>317</v>
       </c>
       <c r="D158" t="n">
-        <v>43.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="159">
@@ -3497,7 +3497,7 @@
         <v>319</v>
       </c>
       <c r="D159" t="n">
-        <v>43.0</v>
+        <v>49.0</v>
       </c>
     </row>
     <row r="160">
@@ -3525,7 +3525,7 @@
         <v>323</v>
       </c>
       <c r="D161" t="n">
-        <v>65.0</v>
+        <v>21.0</v>
       </c>
     </row>
     <row r="162">
@@ -3539,7 +3539,7 @@
         <v>325</v>
       </c>
       <c r="D162" t="n">
-        <v>66.0</v>
+        <v>55.0</v>
       </c>
     </row>
     <row r="163">
@@ -3553,7 +3553,7 @@
         <v>327</v>
       </c>
       <c r="D163" t="n">
-        <v>30.0</v>
+        <v>28.0</v>
       </c>
     </row>
     <row r="164">
@@ -3567,7 +3567,7 @@
         <v>329</v>
       </c>
       <c r="D164" t="n">
-        <v>57.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="165">
@@ -3581,7 +3581,7 @@
         <v>331</v>
       </c>
       <c r="D165" t="n">
-        <v>42.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="166">
@@ -3595,7 +3595,7 @@
         <v>333</v>
       </c>
       <c r="D166" t="n">
-        <v>47.0</v>
+        <v>35.0</v>
       </c>
     </row>
     <row r="167">
@@ -3609,7 +3609,7 @@
         <v>335</v>
       </c>
       <c r="D167" t="n">
-        <v>31.0</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="168">
@@ -3623,7 +3623,7 @@
         <v>337</v>
       </c>
       <c r="D168" t="n">
-        <v>56.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="169">
@@ -3637,7 +3637,7 @@
         <v>339</v>
       </c>
       <c r="D169" t="n">
-        <v>37.0</v>
+        <v>47.0</v>
       </c>
     </row>
     <row r="170">
@@ -3651,7 +3651,7 @@
         <v>341</v>
       </c>
       <c r="D170" t="n">
-        <v>65.0</v>
+        <v>57.0</v>
       </c>
     </row>
     <row r="171">
@@ -3665,7 +3665,7 @@
         <v>343</v>
       </c>
       <c r="D171" t="n">
-        <v>22.0</v>
+        <v>43.0</v>
       </c>
     </row>
     <row r="172">
@@ -3693,7 +3693,7 @@
         <v>347</v>
       </c>
       <c r="D173" t="n">
-        <v>35.0</v>
+        <v>38.0</v>
       </c>
     </row>
     <row r="174">
@@ -3707,7 +3707,7 @@
         <v>349</v>
       </c>
       <c r="D174" t="n">
-        <v>66.0</v>
+        <v>63.0</v>
       </c>
     </row>
     <row r="175">
@@ -3721,7 +3721,7 @@
         <v>351</v>
       </c>
       <c r="D175" t="n">
-        <v>24.0</v>
+        <v>58.0</v>
       </c>
     </row>
     <row r="176">
@@ -3735,7 +3735,7 @@
         <v>353</v>
       </c>
       <c r="D176" t="n">
-        <v>44.0</v>
+        <v>55.0</v>
       </c>
     </row>
     <row r="177">
@@ -3749,7 +3749,7 @@
         <v>355</v>
       </c>
       <c r="D177" t="n">
-        <v>47.0</v>
+        <v>67.0</v>
       </c>
     </row>
     <row r="178">
@@ -3763,7 +3763,7 @@
         <v>357</v>
       </c>
       <c r="D178" t="n">
-        <v>60.0</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="179">
@@ -3777,7 +3777,7 @@
         <v>359</v>
       </c>
       <c r="D179" t="n">
-        <v>40.0</v>
+        <v>43.0</v>
       </c>
     </row>
     <row r="180">
@@ -3791,7 +3791,7 @@
         <v>361</v>
       </c>
       <c r="D180" t="n">
-        <v>21.0</v>
+        <v>45.0</v>
       </c>
     </row>
     <row r="181">
@@ -3805,7 +3805,7 @@
         <v>363</v>
       </c>
       <c r="D181" t="n">
-        <v>38.0</v>
+        <v>65.0</v>
       </c>
     </row>
     <row r="182">
@@ -3819,7 +3819,7 @@
         <v>365</v>
       </c>
       <c r="D182" t="n">
-        <v>29.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="183">
@@ -3833,7 +3833,7 @@
         <v>367</v>
       </c>
       <c r="D183" t="n">
-        <v>50.0</v>
+        <v>40.0</v>
       </c>
     </row>
     <row r="184">
@@ -3847,7 +3847,7 @@
         <v>369</v>
       </c>
       <c r="D184" t="n">
-        <v>59.0</v>
+        <v>39.0</v>
       </c>
     </row>
     <row r="185">
@@ -3861,7 +3861,7 @@
         <v>371</v>
       </c>
       <c r="D185" t="n">
-        <v>60.0</v>
+        <v>31.0</v>
       </c>
     </row>
     <row r="186">
@@ -3875,7 +3875,7 @@
         <v>373</v>
       </c>
       <c r="D186" t="n">
-        <v>37.0</v>
+        <v>19.0</v>
       </c>
     </row>
     <row r="187">
@@ -3889,7 +3889,7 @@
         <v>375</v>
       </c>
       <c r="D187" t="n">
-        <v>29.0</v>
+        <v>63.0</v>
       </c>
     </row>
     <row r="188">
@@ -3903,7 +3903,7 @@
         <v>377</v>
       </c>
       <c r="D188" t="n">
-        <v>26.0</v>
+        <v>49.0</v>
       </c>
     </row>
     <row r="189">
@@ -3917,7 +3917,7 @@
         <v>379</v>
       </c>
       <c r="D189" t="n">
-        <v>25.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="190">
@@ -3931,7 +3931,7 @@
         <v>381</v>
       </c>
       <c r="D190" t="n">
-        <v>27.0</v>
+        <v>31.0</v>
       </c>
     </row>
     <row r="191">
@@ -3945,7 +3945,7 @@
         <v>383</v>
       </c>
       <c r="D191" t="n">
-        <v>51.0</v>
+        <v>55.0</v>
       </c>
     </row>
     <row r="192">
@@ -3959,7 +3959,7 @@
         <v>385</v>
       </c>
       <c r="D192" t="n">
-        <v>35.0</v>
+        <v>44.0</v>
       </c>
     </row>
     <row r="193">
@@ -3973,7 +3973,7 @@
         <v>387</v>
       </c>
       <c r="D193" t="n">
-        <v>44.0</v>
+        <v>51.0</v>
       </c>
     </row>
     <row r="194">
@@ -3987,7 +3987,7 @@
         <v>389</v>
       </c>
       <c r="D194" t="n">
-        <v>52.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="195">
@@ -4001,7 +4001,7 @@
         <v>391</v>
       </c>
       <c r="D195" t="n">
-        <v>63.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="196">
@@ -4015,7 +4015,7 @@
         <v>393</v>
       </c>
       <c r="D196" t="n">
-        <v>19.0</v>
+        <v>42.0</v>
       </c>
     </row>
     <row r="197">
@@ -4029,7 +4029,7 @@
         <v>395</v>
       </c>
       <c r="D197" t="n">
-        <v>23.0</v>
+        <v>37.0</v>
       </c>
     </row>
     <row r="198">
@@ -4043,7 +4043,7 @@
         <v>397</v>
       </c>
       <c r="D198" t="n">
-        <v>39.0</v>
+        <v>26.0</v>
       </c>
     </row>
     <row r="199">
@@ -4057,7 +4057,7 @@
         <v>399</v>
       </c>
       <c r="D199" t="n">
-        <v>52.0</v>
+        <v>36.0</v>
       </c>
     </row>
     <row r="200">
@@ -4071,7 +4071,7 @@
         <v>401</v>
       </c>
       <c r="D200" t="n">
-        <v>56.0</v>
+        <v>53.0</v>
       </c>
     </row>
     <row r="201">
@@ -4085,7 +4085,7 @@
         <v>403</v>
       </c>
       <c r="D201" t="n">
-        <v>24.0</v>
+        <v>32.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>